<commit_message>
put line and candle graph in 1 page
</commit_message>
<xml_diff>
--- a/coinrankingline.xlsx
+++ b/coinrankingline.xlsx
@@ -22,868 +22,868 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>17426.489285913114</t>
-  </si>
-  <si>
-    <t>17426.31968059318</t>
-  </si>
-  <si>
-    <t>17432.365909927816</t>
-  </si>
-  <si>
-    <t>17422.928587502807</t>
-  </si>
-  <si>
-    <t>17441.920482319136</t>
-  </si>
-  <si>
-    <t>17430.197513119718</t>
-  </si>
-  <si>
-    <t>17428.036806945995</t>
-  </si>
-  <si>
-    <t>17443.145665072636</t>
-  </si>
-  <si>
-    <t>17424.924829854917</t>
-  </si>
-  <si>
-    <t>17425.54959127915</t>
-  </si>
-  <si>
-    <t>17431.481488886766</t>
-  </si>
-  <si>
-    <t>17425.591913338165</t>
-  </si>
-  <si>
-    <t>17445.162308282517</t>
-  </si>
-  <si>
-    <t>17420.67435628022</t>
-  </si>
-  <si>
-    <t>17429.976587745237</t>
-  </si>
-  <si>
-    <t>17440.005313792506</t>
-  </si>
-  <si>
-    <t>17435.216304200938</t>
-  </si>
-  <si>
-    <t>17439.096532522926</t>
-  </si>
-  <si>
-    <t>17441.607877622704</t>
-  </si>
-  <si>
-    <t>17444.675503922754</t>
-  </si>
-  <si>
-    <t>17441.35686192538</t>
-  </si>
-  <si>
-    <t>17441.40230185252</t>
-  </si>
-  <si>
-    <t>17457.06502233145</t>
-  </si>
-  <si>
-    <t>17443.0486908213</t>
-  </si>
-  <si>
-    <t>17460.629537312696</t>
-  </si>
-  <si>
-    <t>17457.459054070885</t>
-  </si>
-  <si>
-    <t>17475.347664421057</t>
-  </si>
-  <si>
-    <t>17454.34667407524</t>
-  </si>
-  <si>
-    <t>17480.043702160703</t>
-  </si>
-  <si>
-    <t>17453.766061066966</t>
-  </si>
-  <si>
-    <t>17472.33691564561</t>
-  </si>
-  <si>
-    <t>17453.184933944867</t>
-  </si>
-  <si>
-    <t>17464.73324086529</t>
-  </si>
-  <si>
-    <t>17468.741524068995</t>
-  </si>
-  <si>
-    <t>17473.838656328633</t>
-  </si>
-  <si>
-    <t>17476.744808813823</t>
-  </si>
-  <si>
-    <t>17482.03045586381</t>
-  </si>
-  <si>
-    <t>17462.47143420069</t>
-  </si>
-  <si>
-    <t>17459.78318725558</t>
-  </si>
-  <si>
-    <t>17476.11544505452</t>
-  </si>
-  <si>
-    <t>17459.990752573787</t>
-  </si>
-  <si>
-    <t>17447.771643526856</t>
-  </si>
-  <si>
-    <t>17453.062118378974</t>
-  </si>
-  <si>
-    <t>17441.69036800225</t>
-  </si>
-  <si>
-    <t>17447.417042043497</t>
-  </si>
-  <si>
-    <t>17451.839547420066</t>
-  </si>
-  <si>
-    <t>17448.89854252663</t>
-  </si>
-  <si>
-    <t>17447.141428772007</t>
-  </si>
-  <si>
-    <t>17447.718240581806</t>
-  </si>
-  <si>
-    <t>17440.3309441872</t>
-  </si>
-  <si>
-    <t>17449.39204888274</t>
-  </si>
-  <si>
-    <t>17434.056664622545</t>
-  </si>
-  <si>
-    <t>17449.9674124039</t>
-  </si>
-  <si>
-    <t>17437.39401922746</t>
-  </si>
-  <si>
-    <t>17440.182297239855</t>
-  </si>
-  <si>
-    <t>17431.993487515763</t>
-  </si>
-  <si>
-    <t>17447.114580032943</t>
-  </si>
-  <si>
-    <t>17431.04475263284</t>
-  </si>
-  <si>
-    <t>17439.225259389874</t>
-  </si>
-  <si>
-    <t>17446.33059357636</t>
-  </si>
-  <si>
-    <t>17431.016192647447</t>
-  </si>
-  <si>
-    <t>17445.236553339957</t>
-  </si>
-  <si>
-    <t>17448.36494648703</t>
-  </si>
-  <si>
-    <t>17454.554644111777</t>
-  </si>
-  <si>
-    <t>17449.982816118336</t>
-  </si>
-  <si>
-    <t>17439.687784143847</t>
-  </si>
-  <si>
-    <t>17451.536689366236</t>
-  </si>
-  <si>
-    <t>17445.71605762729</t>
-  </si>
-  <si>
-    <t>17453.1171080667</t>
-  </si>
-  <si>
-    <t>17445.097591060054</t>
-  </si>
-  <si>
-    <t>17446.79531584532</t>
-  </si>
-  <si>
-    <t>17466.896209937746</t>
-  </si>
-  <si>
-    <t>17449.676041551982</t>
-  </si>
-  <si>
-    <t>17479.437891850048</t>
-  </si>
-  <si>
-    <t>17452.77972276831</t>
-  </si>
-  <si>
-    <t>17471.031583505603</t>
-  </si>
-  <si>
-    <t>17457.15130364718</t>
-  </si>
-  <si>
-    <t>17479.570171412975</t>
-  </si>
-  <si>
-    <t>17465.990834194912</t>
-  </si>
-  <si>
-    <t>17460.334597339337</t>
-  </si>
-  <si>
-    <t>17450.22242420014</t>
-  </si>
-  <si>
-    <t>17463.700171155462</t>
-  </si>
-  <si>
-    <t>17444.78164976573</t>
-  </si>
-  <si>
-    <t>17460.82663449306</t>
-  </si>
-  <si>
-    <t>17453.449825374155</t>
-  </si>
-  <si>
-    <t>17461.56627098472</t>
-  </si>
-  <si>
-    <t>17465.733348369522</t>
-  </si>
-  <si>
-    <t>17456.89445155476</t>
-  </si>
-  <si>
-    <t>17449.23622292558</t>
-  </si>
-  <si>
-    <t>17446.907874673157</t>
-  </si>
-  <si>
-    <t>17437.05747842924</t>
-  </si>
-  <si>
-    <t>17455.06777456327</t>
-  </si>
-  <si>
-    <t>17433.96412198383</t>
-  </si>
-  <si>
-    <t>17455.274489996187</t>
-  </si>
-  <si>
-    <t>17430.883799292384</t>
-  </si>
-  <si>
-    <t>17419.986660280225</t>
-  </si>
-  <si>
-    <t>17414.16872198993</t>
-  </si>
-  <si>
-    <t>17424.3741916572</t>
-  </si>
-  <si>
-    <t>17422.836039759055</t>
-  </si>
-  <si>
-    <t>17434.260883777228</t>
-  </si>
-  <si>
-    <t>17416.9566258804</t>
-  </si>
-  <si>
-    <t>17425.627029939053</t>
-  </si>
-  <si>
-    <t>17414.87008341368</t>
-  </si>
-  <si>
-    <t>17414.471887403135</t>
-  </si>
-  <si>
-    <t>17416.174012977655</t>
-  </si>
-  <si>
-    <t>17403.360159773623</t>
-  </si>
-  <si>
-    <t>17417.527046292507</t>
-  </si>
-  <si>
-    <t>17414.606954956504</t>
-  </si>
-  <si>
-    <t>17401.899641950913</t>
-  </si>
-  <si>
-    <t>17403.695928319725</t>
-  </si>
-  <si>
-    <t>17397.935258198217</t>
-  </si>
-  <si>
-    <t>17395.575571716894</t>
-  </si>
-  <si>
-    <t>17385.772618119867</t>
-  </si>
-  <si>
-    <t>17385.756839528876</t>
-  </si>
-  <si>
-    <t>17401.37952145508</t>
-  </si>
-  <si>
-    <t>17342.123555841</t>
-  </si>
-  <si>
-    <t>17369.385573881627</t>
-  </si>
-  <si>
-    <t>17328.86623263935</t>
-  </si>
-  <si>
-    <t>17334.570433922636</t>
-  </si>
-  <si>
-    <t>17326.031072737187</t>
-  </si>
-  <si>
-    <t>17323.50741656222</t>
-  </si>
-  <si>
-    <t>17326.69031114471</t>
-  </si>
-  <si>
-    <t>17318.902501537254</t>
-  </si>
-  <si>
-    <t>17330.028055815226</t>
-  </si>
-  <si>
-    <t>17316.65175796837</t>
-  </si>
-  <si>
-    <t>17337.839289876807</t>
-  </si>
-  <si>
-    <t>17314.888092398556</t>
-  </si>
-  <si>
-    <t>17317.20332356591</t>
-  </si>
-  <si>
-    <t>17314.78967228156</t>
-  </si>
-  <si>
-    <t>17316.10883643534</t>
-  </si>
-  <si>
-    <t>17323.056244903237</t>
-  </si>
-  <si>
-    <t>17327.699883642177</t>
-  </si>
-  <si>
-    <t>17316.43380053404</t>
-  </si>
-  <si>
-    <t>17314.69828060668</t>
-  </si>
-  <si>
-    <t>17328.77719250865</t>
-  </si>
-  <si>
-    <t>17311.41046220501</t>
-  </si>
-  <si>
-    <t>17316.97034702568</t>
-  </si>
-  <si>
-    <t>17311.23944491805</t>
-  </si>
-  <si>
-    <t>17318.96944014582</t>
-  </si>
-  <si>
-    <t>17306.62368064756</t>
-  </si>
-  <si>
-    <t>17337.709375594335</t>
-  </si>
-  <si>
-    <t>17317.265843169556</t>
-  </si>
-  <si>
-    <t>17325.09848434072</t>
-  </si>
-  <si>
-    <t>17314.37144606604</t>
-  </si>
-  <si>
-    <t>17325.163160076274</t>
-  </si>
-  <si>
-    <t>17324.531781918115</t>
-  </si>
-  <si>
-    <t>17303.964042110096</t>
-  </si>
-  <si>
-    <t>17314.667545682325</t>
-  </si>
-  <si>
-    <t>17270.98232497797</t>
-  </si>
-  <si>
-    <t>17316.37387063382</t>
-  </si>
-  <si>
-    <t>17291.148488591283</t>
-  </si>
-  <si>
-    <t>17313.80598909254</t>
-  </si>
-  <si>
-    <t>17321.601474874813</t>
-  </si>
-  <si>
-    <t>17316.25836629766</t>
-  </si>
-  <si>
-    <t>17319.245214586004</t>
-  </si>
-  <si>
-    <t>17301.428639945036</t>
-  </si>
-  <si>
-    <t>17279.687860934835</t>
-  </si>
-  <si>
-    <t>17283.48142189731</t>
-  </si>
-  <si>
-    <t>17281.51964879311</t>
-  </si>
-  <si>
-    <t>17240.18872680268</t>
-  </si>
-  <si>
-    <t>17268.617566873163</t>
-  </si>
-  <si>
-    <t>17249.6030326523</t>
-  </si>
-  <si>
-    <t>17276.64940195365</t>
-  </si>
-  <si>
-    <t>17266.91913970138</t>
-  </si>
-  <si>
-    <t>17245.182558724162</t>
-  </si>
-  <si>
-    <t>17256.046936294693</t>
-  </si>
-  <si>
-    <t>17247.14340184075</t>
-  </si>
-  <si>
-    <t>17270.258826689467</t>
-  </si>
-  <si>
-    <t>17261.849405311794</t>
-  </si>
-  <si>
-    <t>17261.73925538497</t>
-  </si>
-  <si>
-    <t>17246.974805696882</t>
-  </si>
-  <si>
-    <t>17247.23532151749</t>
-  </si>
-  <si>
-    <t>17255.367682895885</t>
-  </si>
-  <si>
-    <t>17234.52351414409</t>
-  </si>
-  <si>
-    <t>17227.379230005477</t>
-  </si>
-  <si>
-    <t>17241.59651687345</t>
-  </si>
-  <si>
-    <t>17255.40116922288</t>
-  </si>
-  <si>
-    <t>17246.271443857506</t>
-  </si>
-  <si>
-    <t>17237.453459914097</t>
-  </si>
-  <si>
-    <t>17253.91377534934</t>
-  </si>
-  <si>
-    <t>17257.03831595126</t>
-  </si>
-  <si>
-    <t>17253.23896232745</t>
-  </si>
-  <si>
-    <t>17249.782290150622</t>
-  </si>
-  <si>
-    <t>17258.770894796482</t>
-  </si>
-  <si>
-    <t>17246.170255406683</t>
-  </si>
-  <si>
-    <t>17271.325667152567</t>
-  </si>
-  <si>
-    <t>17256.331674906196</t>
-  </si>
-  <si>
-    <t>17263.64087235986</t>
-  </si>
-  <si>
-    <t>17269.15430644377</t>
-  </si>
-  <si>
-    <t>17256.465764442735</t>
-  </si>
-  <si>
-    <t>17274.44692762014</t>
-  </si>
-  <si>
-    <t>17287.44431368489</t>
-  </si>
-  <si>
-    <t>17282.830861522256</t>
-  </si>
-  <si>
-    <t>17284.353983496476</t>
-  </si>
-  <si>
-    <t>17268.751865078033</t>
-  </si>
-  <si>
-    <t>17282.644139488468</t>
-  </si>
-  <si>
-    <t>17280.57570672674</t>
-  </si>
-  <si>
-    <t>17273.326101216742</t>
-  </si>
-  <si>
-    <t>17275.819984385562</t>
-  </si>
-  <si>
-    <t>17281.46207030072</t>
-  </si>
-  <si>
-    <t>17288.636749107965</t>
-  </si>
-  <si>
-    <t>17274.321386765165</t>
-  </si>
-  <si>
-    <t>17268.906978404455</t>
-  </si>
-  <si>
-    <t>17272.30056075828</t>
-  </si>
-  <si>
-    <t>17268.135799290565</t>
-  </si>
-  <si>
-    <t>17269.534611044626</t>
-  </si>
-  <si>
-    <t>17271.65104334808</t>
-  </si>
-  <si>
-    <t>17259.64043912045</t>
-  </si>
-  <si>
-    <t>17267.676816593732</t>
-  </si>
-  <si>
-    <t>17248.827146664742</t>
-  </si>
-  <si>
-    <t>17263.134639332126</t>
-  </si>
-  <si>
-    <t>17250.74417913569</t>
-  </si>
-  <si>
-    <t>17248.610571754827</t>
-  </si>
-  <si>
-    <t>17258.20529126799</t>
-  </si>
-  <si>
-    <t>17244.52648293043</t>
-  </si>
-  <si>
-    <t>17263.441560375737</t>
-  </si>
-  <si>
-    <t>17242.416110479695</t>
-  </si>
-  <si>
-    <t>17263.275542959407</t>
-  </si>
-  <si>
-    <t>17234.94657597604</t>
-  </si>
-  <si>
-    <t>17253.880986323107</t>
-  </si>
-  <si>
-    <t>17244.454843448657</t>
-  </si>
-  <si>
-    <t>17256.80084174667</t>
-  </si>
-  <si>
-    <t>17237.559803421205</t>
-  </si>
-  <si>
-    <t>17254.569320208488</t>
-  </si>
-  <si>
-    <t>17240.50262217429</t>
-  </si>
-  <si>
-    <t>17252.654419258262</t>
-  </si>
-  <si>
-    <t>17240.063095679358</t>
-  </si>
-  <si>
-    <t>17237.31130924726</t>
-  </si>
-  <si>
-    <t>17239.295503250152</t>
-  </si>
-  <si>
-    <t>17239.049647704705</t>
-  </si>
-  <si>
-    <t>17254.264559318057</t>
-  </si>
-  <si>
-    <t>17249.746536026134</t>
-  </si>
-  <si>
-    <t>17236.19574050662</t>
-  </si>
-  <si>
-    <t>17235.437217852217</t>
-  </si>
-  <si>
-    <t>17238.8864555186</t>
-  </si>
-  <si>
-    <t>17244.617250876436</t>
-  </si>
-  <si>
-    <t>17239.71206294703</t>
-  </si>
-  <si>
-    <t>17234.353227895564</t>
-  </si>
-  <si>
-    <t>17215.459779662106</t>
-  </si>
-  <si>
-    <t>17218.978157218047</t>
-  </si>
-  <si>
-    <t>17217.415407953842</t>
-  </si>
-  <si>
-    <t>17221.51449000356</t>
-  </si>
-  <si>
-    <t>17216.054064843145</t>
-  </si>
-  <si>
-    <t>17214.17203910927</t>
-  </si>
-  <si>
-    <t>17209.10890347184</t>
-  </si>
-  <si>
-    <t>17206.67133962618</t>
-  </si>
-  <si>
-    <t>17212.31140089807</t>
-  </si>
-  <si>
-    <t>17205.175647409844</t>
-  </si>
-  <si>
-    <t>17209.59626153872</t>
-  </si>
-  <si>
-    <t>17202.192415599493</t>
-  </si>
-  <si>
-    <t>17201.26718510966</t>
-  </si>
-  <si>
-    <t>17204.760186828855</t>
-  </si>
-  <si>
-    <t>17196.00694860244</t>
-  </si>
-  <si>
-    <t>17196.957431605904</t>
-  </si>
-  <si>
-    <t>17207.93004286377</t>
-  </si>
-  <si>
-    <t>17199.877972021288</t>
-  </si>
-  <si>
-    <t>17211.08366198878</t>
-  </si>
-  <si>
-    <t>17198.170657732906</t>
-  </si>
-  <si>
-    <t>17213.997038480727</t>
-  </si>
-  <si>
-    <t>17207.85559447794</t>
-  </si>
-  <si>
-    <t>17208.748519061402</t>
-  </si>
-  <si>
-    <t>17215.41120830141</t>
-  </si>
-  <si>
-    <t>17215.23583159277</t>
-  </si>
-  <si>
-    <t>17204.31053398349</t>
-  </si>
-  <si>
-    <t>17208.58857864455</t>
-  </si>
-  <si>
-    <t>17210.342809519727</t>
-  </si>
-  <si>
-    <t>17217.250797553148</t>
-  </si>
-  <si>
-    <t>17212.873681545443</t>
-  </si>
-  <si>
-    <t>17213.695700372064</t>
-  </si>
-  <si>
-    <t>17206.508222229448</t>
-  </si>
-  <si>
-    <t>17216.588810546156</t>
-  </si>
-  <si>
-    <t>17209.15051437555</t>
-  </si>
-  <si>
-    <t>17208.39005881617</t>
-  </si>
-  <si>
-    <t>17202.044757649437</t>
-  </si>
-  <si>
-    <t>17209.326561033227</t>
-  </si>
-  <si>
-    <t>17201.37800107795</t>
-  </si>
-  <si>
-    <t>17202.539553533636</t>
-  </si>
-  <si>
-    <t>17201.934177640065</t>
-  </si>
-  <si>
-    <t>17205.798835628124</t>
-  </si>
-  <si>
-    <t>17211.235151072768</t>
-  </si>
-  <si>
-    <t>17206.869459308335</t>
-  </si>
-  <si>
-    <t>17208.386778524928</t>
-  </si>
-  <si>
-    <t>17210.8675593013</t>
-  </si>
-  <si>
-    <t>17200.8717607514</t>
-  </si>
-  <si>
-    <t>17205.984109879093</t>
-  </si>
-  <si>
-    <t>17191.355905284378</t>
-  </si>
-  <si>
-    <t>17216.777447367796</t>
-  </si>
-  <si>
-    <t>17194.87915539834</t>
+    <t>20949.31774448195</t>
+  </si>
+  <si>
+    <t>20935.062649480013</t>
+  </si>
+  <si>
+    <t>20931.615804486522</t>
+  </si>
+  <si>
+    <t>20918.20940219982</t>
+  </si>
+  <si>
+    <t>20882.412859350814</t>
+  </si>
+  <si>
+    <t>20886.47783247173</t>
+  </si>
+  <si>
+    <t>20863.98640378465</t>
+  </si>
+  <si>
+    <t>20892.64709271599</t>
+  </si>
+  <si>
+    <t>20854.09732229254</t>
+  </si>
+  <si>
+    <t>20879.58263644923</t>
+  </si>
+  <si>
+    <t>20852.354626886576</t>
+  </si>
+  <si>
+    <t>20869.059380897444</t>
+  </si>
+  <si>
+    <t>20889.53755390575</t>
+  </si>
+  <si>
+    <t>20851.38424592719</t>
+  </si>
+  <si>
+    <t>20856.156709017505</t>
+  </si>
+  <si>
+    <t>20900.90030147438</t>
+  </si>
+  <si>
+    <t>20828.478709204097</t>
+  </si>
+  <si>
+    <t>20878.891320843864</t>
+  </si>
+  <si>
+    <t>20862.58341211068</t>
+  </si>
+  <si>
+    <t>20889.346656402424</t>
+  </si>
+  <si>
+    <t>20852.192984105754</t>
+  </si>
+  <si>
+    <t>20876.99430315978</t>
+  </si>
+  <si>
+    <t>20859.839384817347</t>
+  </si>
+  <si>
+    <t>20858.74172264787</t>
+  </si>
+  <si>
+    <t>20826.22037503476</t>
+  </si>
+  <si>
+    <t>20809.36915291311</t>
+  </si>
+  <si>
+    <t>20806.417438222135</t>
+  </si>
+  <si>
+    <t>20833.274923614215</t>
+  </si>
+  <si>
+    <t>20800.73891854358</t>
+  </si>
+  <si>
+    <t>20824.1409214702</t>
+  </si>
+  <si>
+    <t>20769.42311723904</t>
+  </si>
+  <si>
+    <t>20771.60646012688</t>
+  </si>
+  <si>
+    <t>20741.842428278473</t>
+  </si>
+  <si>
+    <t>20759.998024084536</t>
+  </si>
+  <si>
+    <t>20759.015676463187</t>
+  </si>
+  <si>
+    <t>20738.230383335467</t>
+  </si>
+  <si>
+    <t>20735.524072454744</t>
+  </si>
+  <si>
+    <t>20716.65483750799</t>
+  </si>
+  <si>
+    <t>20693.335257609087</t>
+  </si>
+  <si>
+    <t>20705.072769465296</t>
+  </si>
+  <si>
+    <t>20703.84123818575</t>
+  </si>
+  <si>
+    <t>20689.315240281492</t>
+  </si>
+  <si>
+    <t>20696.418933458568</t>
+  </si>
+  <si>
+    <t>20692.11016647735</t>
+  </si>
+  <si>
+    <t>20694.104955766743</t>
+  </si>
+  <si>
+    <t>20693.199443751484</t>
+  </si>
+  <si>
+    <t>20704.827255858658</t>
+  </si>
+  <si>
+    <t>20710.425662826292</t>
+  </si>
+  <si>
+    <t>20722.518242056114</t>
+  </si>
+  <si>
+    <t>20692.42566690557</t>
+  </si>
+  <si>
+    <t>20692.75395733665</t>
+  </si>
+  <si>
+    <t>20688.965914122036</t>
+  </si>
+  <si>
+    <t>20672.583696710895</t>
+  </si>
+  <si>
+    <t>20700.635187499734</t>
+  </si>
+  <si>
+    <t>20667.76701003743</t>
+  </si>
+  <si>
+    <t>20676.817486723514</t>
+  </si>
+  <si>
+    <t>20680.383204728198</t>
+  </si>
+  <si>
+    <t>20654.63397438002</t>
+  </si>
+  <si>
+    <t>20687.49377678753</t>
+  </si>
+  <si>
+    <t>20671.708709936902</t>
+  </si>
+  <si>
+    <t>20685.95005281452</t>
+  </si>
+  <si>
+    <t>20639.491133927993</t>
+  </si>
+  <si>
+    <t>20672.318947404878</t>
+  </si>
+  <si>
+    <t>20660.9308017286</t>
+  </si>
+  <si>
+    <t>20665.044280022485</t>
+  </si>
+  <si>
+    <t>20661.861432396287</t>
+  </si>
+  <si>
+    <t>20658.201360160092</t>
+  </si>
+  <si>
+    <t>20679.595493599736</t>
+  </si>
+  <si>
+    <t>20684.455108794566</t>
+  </si>
+  <si>
+    <t>20676.7150535547</t>
+  </si>
+  <si>
+    <t>20658.2365509765</t>
+  </si>
+  <si>
+    <t>20678.919497943083</t>
+  </si>
+  <si>
+    <t>20664.949073579326</t>
+  </si>
+  <si>
+    <t>20664.1355142</t>
+  </si>
+  <si>
+    <t>20689.633929374006</t>
+  </si>
+  <si>
+    <t>20681.340337794834</t>
+  </si>
+  <si>
+    <t>20671.99411683978</t>
+  </si>
+  <si>
+    <t>20683.557332917208</t>
+  </si>
+  <si>
+    <t>20665.41028106282</t>
+  </si>
+  <si>
+    <t>20677.050915217264</t>
+  </si>
+  <si>
+    <t>20699.932619484396</t>
+  </si>
+  <si>
+    <t>20704.138158023277</t>
+  </si>
+  <si>
+    <t>20694.129927507078</t>
+  </si>
+  <si>
+    <t>20678.430526299493</t>
+  </si>
+  <si>
+    <t>20694.0417430734</t>
+  </si>
+  <si>
+    <t>20690.87927110508</t>
+  </si>
+  <si>
+    <t>20681.807731728924</t>
+  </si>
+  <si>
+    <t>20694.8392759862</t>
+  </si>
+  <si>
+    <t>20666.961317472098</t>
+  </si>
+  <si>
+    <t>20701.91485321567</t>
+  </si>
+  <si>
+    <t>20680.985242927938</t>
+  </si>
+  <si>
+    <t>20675.458198204728</t>
+  </si>
+  <si>
+    <t>20698.770016922008</t>
+  </si>
+  <si>
+    <t>20641.00603211735</t>
+  </si>
+  <si>
+    <t>20636.947931931743</t>
+  </si>
+  <si>
+    <t>20640.561333804962</t>
+  </si>
+  <si>
+    <t>20631.812511008033</t>
+  </si>
+  <si>
+    <t>20662.600445001357</t>
+  </si>
+  <si>
+    <t>20642.642614998218</t>
+  </si>
+  <si>
+    <t>20657.28247977816</t>
+  </si>
+  <si>
+    <t>20662.65727544866</t>
+  </si>
+  <si>
+    <t>20661.647917167295</t>
+  </si>
+  <si>
+    <t>20625.918800104886</t>
+  </si>
+  <si>
+    <t>20665.169958278333</t>
+  </si>
+  <si>
+    <t>20670.32122825946</t>
+  </si>
+  <si>
+    <t>20658.07477184523</t>
+  </si>
+  <si>
+    <t>20692.222713849405</t>
+  </si>
+  <si>
+    <t>20694.227649047705</t>
+  </si>
+  <si>
+    <t>20717.42818573868</t>
+  </si>
+  <si>
+    <t>20698.546224693393</t>
+  </si>
+  <si>
+    <t>20705.149273553696</t>
+  </si>
+  <si>
+    <t>20698.352621704766</t>
+  </si>
+  <si>
+    <t>20726.545569529553</t>
+  </si>
+  <si>
+    <t>20732.308434360428</t>
+  </si>
+  <si>
+    <t>20742.621286935282</t>
+  </si>
+  <si>
+    <t>20725.98949370872</t>
+  </si>
+  <si>
+    <t>20740.886158328172</t>
+  </si>
+  <si>
+    <t>20721.70594136364</t>
+  </si>
+  <si>
+    <t>20741.010734817315</t>
+  </si>
+  <si>
+    <t>20727.953431841877</t>
+  </si>
+  <si>
+    <t>20730.996582513162</t>
+  </si>
+  <si>
+    <t>20735.686563552477</t>
+  </si>
+  <si>
+    <t>20726.142763593823</t>
+  </si>
+  <si>
+    <t>20730.29731339886</t>
+  </si>
+  <si>
+    <t>20728.18639296621</t>
+  </si>
+  <si>
+    <t>20711.604008088612</t>
+  </si>
+  <si>
+    <t>20726.304740357606</t>
+  </si>
+  <si>
+    <t>20718.175569847892</t>
+  </si>
+  <si>
+    <t>20727.351124415007</t>
+  </si>
+  <si>
+    <t>20737.671952123528</t>
+  </si>
+  <si>
+    <t>20725.63255493763</t>
+  </si>
+  <si>
+    <t>20742.414582509904</t>
+  </si>
+  <si>
+    <t>20735.169885627485</t>
+  </si>
+  <si>
+    <t>20759.20065575835</t>
+  </si>
+  <si>
+    <t>20758.916022577116</t>
+  </si>
+  <si>
+    <t>20748.210567402206</t>
+  </si>
+  <si>
+    <t>20738.561746776104</t>
+  </si>
+  <si>
+    <t>20722.575842768976</t>
+  </si>
+  <si>
+    <t>20732.80475543056</t>
+  </si>
+  <si>
+    <t>20730.357165487665</t>
+  </si>
+  <si>
+    <t>20731.23469741569</t>
+  </si>
+  <si>
+    <t>20731.127779604958</t>
+  </si>
+  <si>
+    <t>20726.55807546686</t>
+  </si>
+  <si>
+    <t>20726.59302245157</t>
+  </si>
+  <si>
+    <t>20736.912025260215</t>
+  </si>
+  <si>
+    <t>20733.39897170137</t>
+  </si>
+  <si>
+    <t>20736.20628534306</t>
+  </si>
+  <si>
+    <t>20736.502491668725</t>
+  </si>
+  <si>
+    <t>20745.44251337991</t>
+  </si>
+  <si>
+    <t>20716.176388239168</t>
+  </si>
+  <si>
+    <t>20695.621997658454</t>
+  </si>
+  <si>
+    <t>20695.799478043777</t>
+  </si>
+  <si>
+    <t>20695.851007199504</t>
+  </si>
+  <si>
+    <t>20699.200261935443</t>
+  </si>
+  <si>
+    <t>20703.320340339757</t>
+  </si>
+  <si>
+    <t>20697.45976554703</t>
+  </si>
+  <si>
+    <t>20734.203165264375</t>
+  </si>
+  <si>
+    <t>20719.909345993474</t>
+  </si>
+  <si>
+    <t>20705.501106708605</t>
+  </si>
+  <si>
+    <t>20713.605571458702</t>
+  </si>
+  <si>
+    <t>20715.53379281618</t>
+  </si>
+  <si>
+    <t>20715.89565777028</t>
+  </si>
+  <si>
+    <t>20713.15103811722</t>
+  </si>
+  <si>
+    <t>20708.24380642493</t>
+  </si>
+  <si>
+    <t>20704.043206505554</t>
+  </si>
+  <si>
+    <t>20697.274862835453</t>
+  </si>
+  <si>
+    <t>20690.5410725031</t>
+  </si>
+  <si>
+    <t>20689.50548458013</t>
+  </si>
+  <si>
+    <t>20675.436228017483</t>
+  </si>
+  <si>
+    <t>20688.80616826993</t>
+  </si>
+  <si>
+    <t>20668.28906441839</t>
+  </si>
+  <si>
+    <t>20662.846756449097</t>
+  </si>
+  <si>
+    <t>20670.356132521683</t>
+  </si>
+  <si>
+    <t>20714.52462683718</t>
+  </si>
+  <si>
+    <t>20672.797178173365</t>
+  </si>
+  <si>
+    <t>20738.4560491957</t>
+  </si>
+  <si>
+    <t>20698.812139489688</t>
+  </si>
+  <si>
+    <t>20721.53452328185</t>
+  </si>
+  <si>
+    <t>20725.29096471515</t>
+  </si>
+  <si>
+    <t>20756.55357718201</t>
+  </si>
+  <si>
+    <t>20711.06441789404</t>
+  </si>
+  <si>
+    <t>20759.356768239777</t>
+  </si>
+  <si>
+    <t>20765.724848668815</t>
+  </si>
+  <si>
+    <t>20745.40923036501</t>
+  </si>
+  <si>
+    <t>20759.385664469217</t>
+  </si>
+  <si>
+    <t>20740.340188036967</t>
+  </si>
+  <si>
+    <t>20761.6679527366</t>
+  </si>
+  <si>
+    <t>20787.260301161637</t>
+  </si>
+  <si>
+    <t>20772.597571905917</t>
+  </si>
+  <si>
+    <t>20764.29373129274</t>
+  </si>
+  <si>
+    <t>20781.409592384734</t>
+  </si>
+  <si>
+    <t>20763.995100703687</t>
+  </si>
+  <si>
+    <t>20762.45291608892</t>
+  </si>
+  <si>
+    <t>20773.76723537301</t>
+  </si>
+  <si>
+    <t>20720.943396415078</t>
+  </si>
+  <si>
+    <t>20770.659008698487</t>
+  </si>
+  <si>
+    <t>20725.42112802626</t>
+  </si>
+  <si>
+    <t>20772.361087358633</t>
+  </si>
+  <si>
+    <t>20760.59004054809</t>
+  </si>
+  <si>
+    <t>20786.04306889617</t>
+  </si>
+  <si>
+    <t>20807.06279054836</t>
+  </si>
+  <si>
+    <t>20755.405019867972</t>
+  </si>
+  <si>
+    <t>20862.276168637254</t>
+  </si>
+  <si>
+    <t>20726.112100928527</t>
+  </si>
+  <si>
+    <t>20827.66772050199</t>
+  </si>
+  <si>
+    <t>20724.036335448953</t>
+  </si>
+  <si>
+    <t>20876.297038055938</t>
+  </si>
+  <si>
+    <t>20923.0740922987</t>
+  </si>
+  <si>
+    <t>20908.48520032565</t>
+  </si>
+  <si>
+    <t>20886.898903824273</t>
+  </si>
+  <si>
+    <t>20991.769856200804</t>
+  </si>
+  <si>
+    <t>20890.39295133414</t>
+  </si>
+  <si>
+    <t>20915.151767042615</t>
+  </si>
+  <si>
+    <t>20943.087824080707</t>
+  </si>
+  <si>
+    <t>20944.76390197644</t>
+  </si>
+  <si>
+    <t>20974.606544797818</t>
+  </si>
+  <si>
+    <t>20956.286837676842</t>
+  </si>
+  <si>
+    <t>20965.703291275953</t>
+  </si>
+  <si>
+    <t>20967.837850586584</t>
+  </si>
+  <si>
+    <t>20962.687837084814</t>
+  </si>
+  <si>
+    <t>20919.444162653137</t>
+  </si>
+  <si>
+    <t>20962.027546404304</t>
+  </si>
+  <si>
+    <t>20893.094083735417</t>
+  </si>
+  <si>
+    <t>20948.992336062747</t>
+  </si>
+  <si>
+    <t>20905.90795399405</t>
+  </si>
+  <si>
+    <t>20923.716725017974</t>
+  </si>
+  <si>
+    <t>20878.613859290595</t>
+  </si>
+  <si>
+    <t>20872.761709299604</t>
+  </si>
+  <si>
+    <t>20872.310004669485</t>
+  </si>
+  <si>
+    <t>20864.48546495512</t>
+  </si>
+  <si>
+    <t>20851.206261251606</t>
+  </si>
+  <si>
+    <t>20864.628825516913</t>
+  </si>
+  <si>
+    <t>20843.515892641823</t>
+  </si>
+  <si>
+    <t>20862.10669983968</t>
+  </si>
+  <si>
+    <t>20829.86239039909</t>
+  </si>
+  <si>
+    <t>20847.62715499543</t>
+  </si>
+  <si>
+    <t>20874.314923422273</t>
+  </si>
+  <si>
+    <t>20826.30809299332</t>
+  </si>
+  <si>
+    <t>20854.797121043997</t>
+  </si>
+  <si>
+    <t>20846.363093674405</t>
+  </si>
+  <si>
+    <t>20844.197365184056</t>
+  </si>
+  <si>
+    <t>20854.481737252154</t>
+  </si>
+  <si>
+    <t>20831.377552600094</t>
+  </si>
+  <si>
+    <t>20840.637049750938</t>
+  </si>
+  <si>
+    <t>20869.110639198967</t>
+  </si>
+  <si>
+    <t>20851.679065429507</t>
+  </si>
+  <si>
+    <t>20874.43786065183</t>
+  </si>
+  <si>
+    <t>20806.941484403014</t>
+  </si>
+  <si>
+    <t>20832.73588236277</t>
+  </si>
+  <si>
+    <t>20797.308815447817</t>
+  </si>
+  <si>
+    <t>20793.892379445646</t>
+  </si>
+  <si>
+    <t>20800.378185860664</t>
+  </si>
+  <si>
+    <t>20786.136140016857</t>
+  </si>
+  <si>
+    <t>20786.32939014631</t>
+  </si>
+  <si>
+    <t>20759.779824160887</t>
+  </si>
+  <si>
+    <t>20757.78484615255</t>
+  </si>
+  <si>
+    <t>20789.001632577485</t>
+  </si>
+  <si>
+    <t>20756.65766064941</t>
+  </si>
+  <si>
+    <t>20770.195125667266</t>
+  </si>
+  <si>
+    <t>20748.58985344208</t>
+  </si>
+  <si>
+    <t>20796.908228699747</t>
+  </si>
+  <si>
+    <t>20720.39443875546</t>
+  </si>
+  <si>
+    <t>20796.431949315527</t>
+  </si>
+  <si>
+    <t>20789.74225310135</t>
+  </si>
+  <si>
+    <t>20768.303563432626</t>
+  </si>
+  <si>
+    <t>20763.42673381451</t>
+  </si>
+  <si>
+    <t>20779.146536950117</t>
+  </si>
+  <si>
+    <t>20764.633382031985</t>
+  </si>
+  <si>
+    <t>20763.235719893608</t>
+  </si>
+  <si>
+    <t>20732.779139518374</t>
+  </si>
+  <si>
+    <t>20732.289059115064</t>
+  </si>
+  <si>
+    <t>20739.00267651428</t>
+  </si>
+  <si>
+    <t>20741.57546111627</t>
+  </si>
+  <si>
+    <t>20749.001396915155</t>
+  </si>
+  <si>
+    <t>20725.112974995045</t>
+  </si>
+  <si>
+    <t>20749.68143601495</t>
+  </si>
+  <si>
+    <t>20729.34998793227</t>
+  </si>
+  <si>
+    <t>20740.124204274372</t>
+  </si>
+  <si>
+    <t>20704.825475199577</t>
+  </si>
+  <si>
+    <t>20718.423557595183</t>
+  </si>
+  <si>
+    <t>20740.866957192058</t>
+  </si>
+  <si>
+    <t>20743.664486594113</t>
+  </si>
+  <si>
+    <t>20724.149402213123</t>
+  </si>
+  <si>
+    <t>20782.35654436419</t>
+  </si>
+  <si>
+    <t>20770.353890585786</t>
+  </si>
+  <si>
+    <t>20754.518115152816</t>
+  </si>
+  <si>
+    <t>20822.29292595936</t>
+  </si>
+  <si>
+    <t>20813.058098778823</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1267,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2">
-        <v>44937.46180555555</v>
+        <v>44942.02777777778</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1278,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>44937.45833333334</v>
+        <v>44942.02430555555</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1289,7 +1289,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2">
-        <v>44937.45486111111</v>
+        <v>44942.02083333334</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1300,7 +1300,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="2">
-        <v>44937.45138888889</v>
+        <v>44942.01736111111</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1311,7 +1311,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="2">
-        <v>44937.44791666666</v>
+        <v>44942.01388888889</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1322,7 +1322,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="2">
-        <v>44937.44444444445</v>
+        <v>44942.01041666666</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1333,7 +1333,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="2">
-        <v>44937.44097222222</v>
+        <v>44942.00694444445</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1344,7 +1344,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="2">
-        <v>44937.4375</v>
+        <v>44942.00347222222</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1355,7 +1355,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="2">
-        <v>44937.43402777778</v>
+        <v>44942</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1366,7 +1366,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="2">
-        <v>44937.43055555555</v>
+        <v>44941.99652777778</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1377,7 +1377,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2">
-        <v>44937.42708333334</v>
+        <v>44941.99305555555</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1388,7 +1388,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="2">
-        <v>44937.42361111111</v>
+        <v>44941.98958333334</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1399,7 +1399,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="2">
-        <v>44937.42013888889</v>
+        <v>44941.98611111111</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1410,7 +1410,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="2">
-        <v>44937.41666666666</v>
+        <v>44941.98263888889</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1421,7 +1421,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="2">
-        <v>44937.41319444445</v>
+        <v>44941.97916666666</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1432,7 +1432,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="2">
-        <v>44937.40972222222</v>
+        <v>44941.97569444445</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1443,7 +1443,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="2">
-        <v>44937.40625</v>
+        <v>44941.97222222222</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1454,7 +1454,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="2">
-        <v>44937.40277777778</v>
+        <v>44941.96875</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1465,7 +1465,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="2">
-        <v>44937.39930555555</v>
+        <v>44941.96527777778</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1476,7 +1476,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="2">
-        <v>44937.39583333334</v>
+        <v>44941.96180555555</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1487,7 +1487,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="2">
-        <v>44937.39236111111</v>
+        <v>44941.95833333334</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1498,7 +1498,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="2">
-        <v>44937.38888888889</v>
+        <v>44941.95486111111</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1509,7 +1509,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="2">
-        <v>44937.38541666666</v>
+        <v>44941.95138888889</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1520,7 +1520,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="2">
-        <v>44937.38194444445</v>
+        <v>44941.94791666666</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1531,7 +1531,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="2">
-        <v>44937.37847222222</v>
+        <v>44941.94444444445</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1542,7 +1542,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="2">
-        <v>44937.375</v>
+        <v>44941.94097222222</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1553,7 +1553,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="2">
-        <v>44937.37152777778</v>
+        <v>44941.9375</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1564,7 +1564,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="2">
-        <v>44937.36805555555</v>
+        <v>44941.93402777778</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1575,7 +1575,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="2">
-        <v>44937.36458333334</v>
+        <v>44941.93055555555</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1586,7 +1586,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="2">
-        <v>44937.36111111111</v>
+        <v>44941.92708333334</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1597,7 +1597,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="2">
-        <v>44937.35763888889</v>
+        <v>44941.92361111111</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1608,7 +1608,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="2">
-        <v>44937.35416666666</v>
+        <v>44941.92013888889</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1619,7 +1619,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="2">
-        <v>44937.35069444445</v>
+        <v>44941.91666666666</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1630,7 +1630,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="2">
-        <v>44937.34722222222</v>
+        <v>44941.91319444445</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1641,7 +1641,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="2">
-        <v>44937.34375</v>
+        <v>44941.90972222222</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1652,7 +1652,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="2">
-        <v>44937.34027777778</v>
+        <v>44941.90625</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1663,7 +1663,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="2">
-        <v>44937.33680555555</v>
+        <v>44941.90277777778</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1674,7 +1674,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="2">
-        <v>44937.33333333334</v>
+        <v>44941.89930555555</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1685,7 +1685,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="2">
-        <v>44937.32986111111</v>
+        <v>44941.89583333334</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1696,7 +1696,7 @@
         <v>41</v>
       </c>
       <c r="C41" s="2">
-        <v>44937.32638888889</v>
+        <v>44941.89236111111</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1707,7 +1707,7 @@
         <v>42</v>
       </c>
       <c r="C42" s="2">
-        <v>44937.32291666666</v>
+        <v>44941.88888888889</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1718,7 +1718,7 @@
         <v>43</v>
       </c>
       <c r="C43" s="2">
-        <v>44937.31944444445</v>
+        <v>44941.88541666666</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1729,7 +1729,7 @@
         <v>44</v>
       </c>
       <c r="C44" s="2">
-        <v>44937.31597222222</v>
+        <v>44941.88194444445</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1740,7 +1740,7 @@
         <v>45</v>
       </c>
       <c r="C45" s="2">
-        <v>44937.3125</v>
+        <v>44941.87847222222</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1751,7 +1751,7 @@
         <v>46</v>
       </c>
       <c r="C46" s="2">
-        <v>44937.30902777778</v>
+        <v>44941.875</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1762,7 +1762,7 @@
         <v>47</v>
       </c>
       <c r="C47" s="2">
-        <v>44937.30555555555</v>
+        <v>44941.87152777778</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1773,7 +1773,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="2">
-        <v>44937.30208333334</v>
+        <v>44941.86805555555</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1784,7 +1784,7 @@
         <v>49</v>
       </c>
       <c r="C49" s="2">
-        <v>44937.29861111111</v>
+        <v>44941.86458333334</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1795,7 +1795,7 @@
         <v>50</v>
       </c>
       <c r="C50" s="2">
-        <v>44937.29513888889</v>
+        <v>44941.86111111111</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1806,7 +1806,7 @@
         <v>51</v>
       </c>
       <c r="C51" s="2">
-        <v>44937.29166666666</v>
+        <v>44941.85763888889</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1817,7 +1817,7 @@
         <v>52</v>
       </c>
       <c r="C52" s="2">
-        <v>44937.28819444445</v>
+        <v>44941.85416666666</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1828,7 +1828,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="2">
-        <v>44937.28472222222</v>
+        <v>44941.85069444445</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1839,7 +1839,7 @@
         <v>54</v>
       </c>
       <c r="C54" s="2">
-        <v>44937.28125</v>
+        <v>44941.84722222222</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1850,7 +1850,7 @@
         <v>55</v>
       </c>
       <c r="C55" s="2">
-        <v>44937.27777777778</v>
+        <v>44941.84375</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1861,7 +1861,7 @@
         <v>56</v>
       </c>
       <c r="C56" s="2">
-        <v>44937.27430555555</v>
+        <v>44941.84027777778</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1872,7 +1872,7 @@
         <v>57</v>
       </c>
       <c r="C57" s="2">
-        <v>44937.27083333334</v>
+        <v>44941.83680555555</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1883,7 +1883,7 @@
         <v>58</v>
       </c>
       <c r="C58" s="2">
-        <v>44937.26736111111</v>
+        <v>44941.83333333334</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1894,7 +1894,7 @@
         <v>59</v>
       </c>
       <c r="C59" s="2">
-        <v>44937.26388888889</v>
+        <v>44941.82986111111</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1905,7 +1905,7 @@
         <v>60</v>
       </c>
       <c r="C60" s="2">
-        <v>44937.26041666666</v>
+        <v>44941.82638888889</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1916,7 +1916,7 @@
         <v>61</v>
       </c>
       <c r="C61" s="2">
-        <v>44937.25694444445</v>
+        <v>44941.82291666666</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1927,7 +1927,7 @@
         <v>62</v>
       </c>
       <c r="C62" s="2">
-        <v>44937.25347222222</v>
+        <v>44941.81944444445</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1938,7 +1938,7 @@
         <v>63</v>
       </c>
       <c r="C63" s="2">
-        <v>44937.25</v>
+        <v>44941.81597222222</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1949,7 +1949,7 @@
         <v>64</v>
       </c>
       <c r="C64" s="2">
-        <v>44937.24652777778</v>
+        <v>44941.8125</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1960,7 +1960,7 @@
         <v>65</v>
       </c>
       <c r="C65" s="2">
-        <v>44937.24305555555</v>
+        <v>44941.80902777778</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1971,7 +1971,7 @@
         <v>66</v>
       </c>
       <c r="C66" s="2">
-        <v>44937.23958333334</v>
+        <v>44941.80555555555</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1982,7 +1982,7 @@
         <v>67</v>
       </c>
       <c r="C67" s="2">
-        <v>44937.23611111111</v>
+        <v>44941.80208333334</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1993,7 +1993,7 @@
         <v>68</v>
       </c>
       <c r="C68" s="2">
-        <v>44937.23263888889</v>
+        <v>44941.79861111111</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2004,7 +2004,7 @@
         <v>69</v>
       </c>
       <c r="C69" s="2">
-        <v>44937.22916666666</v>
+        <v>44941.79513888889</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2015,7 +2015,7 @@
         <v>70</v>
       </c>
       <c r="C70" s="2">
-        <v>44937.22569444445</v>
+        <v>44941.79166666666</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2026,7 +2026,7 @@
         <v>71</v>
       </c>
       <c r="C71" s="2">
-        <v>44937.22222222222</v>
+        <v>44941.78819444445</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2037,7 +2037,7 @@
         <v>72</v>
       </c>
       <c r="C72" s="2">
-        <v>44937.21875</v>
+        <v>44941.78472222222</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2048,7 +2048,7 @@
         <v>73</v>
       </c>
       <c r="C73" s="2">
-        <v>44937.21527777778</v>
+        <v>44941.78125</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2059,7 +2059,7 @@
         <v>74</v>
       </c>
       <c r="C74" s="2">
-        <v>44937.21180555555</v>
+        <v>44941.77777777778</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2070,7 +2070,7 @@
         <v>75</v>
       </c>
       <c r="C75" s="2">
-        <v>44937.20833333334</v>
+        <v>44941.77430555555</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2081,7 +2081,7 @@
         <v>76</v>
       </c>
       <c r="C76" s="2">
-        <v>44937.20486111111</v>
+        <v>44941.77083333334</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2092,7 +2092,7 @@
         <v>77</v>
       </c>
       <c r="C77" s="2">
-        <v>44937.20138888889</v>
+        <v>44941.76736111111</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2103,7 +2103,7 @@
         <v>78</v>
       </c>
       <c r="C78" s="2">
-        <v>44937.19791666666</v>
+        <v>44941.76388888889</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2114,7 +2114,7 @@
         <v>79</v>
       </c>
       <c r="C79" s="2">
-        <v>44937.19444444445</v>
+        <v>44941.76041666666</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2125,7 +2125,7 @@
         <v>80</v>
       </c>
       <c r="C80" s="2">
-        <v>44937.19097222222</v>
+        <v>44941.75694444445</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2136,7 +2136,7 @@
         <v>81</v>
       </c>
       <c r="C81" s="2">
-        <v>44937.1875</v>
+        <v>44941.75347222222</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2147,7 +2147,7 @@
         <v>82</v>
       </c>
       <c r="C82" s="2">
-        <v>44937.18402777778</v>
+        <v>44941.75</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2158,7 +2158,7 @@
         <v>83</v>
       </c>
       <c r="C83" s="2">
-        <v>44937.18055555555</v>
+        <v>44941.74652777778</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2169,7 +2169,7 @@
         <v>84</v>
       </c>
       <c r="C84" s="2">
-        <v>44937.17708333334</v>
+        <v>44941.74305555555</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2180,7 +2180,7 @@
         <v>85</v>
       </c>
       <c r="C85" s="2">
-        <v>44937.17361111111</v>
+        <v>44941.73958333334</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2191,7 +2191,7 @@
         <v>86</v>
       </c>
       <c r="C86" s="2">
-        <v>44937.17013888889</v>
+        <v>44941.73611111111</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2202,7 +2202,7 @@
         <v>87</v>
       </c>
       <c r="C87" s="2">
-        <v>44937.16666666666</v>
+        <v>44941.73263888889</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2213,7 +2213,7 @@
         <v>88</v>
       </c>
       <c r="C88" s="2">
-        <v>44937.16319444445</v>
+        <v>44941.72916666666</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2224,7 +2224,7 @@
         <v>89</v>
       </c>
       <c r="C89" s="2">
-        <v>44937.15972222222</v>
+        <v>44941.72569444445</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2235,7 +2235,7 @@
         <v>90</v>
       </c>
       <c r="C90" s="2">
-        <v>44937.15625</v>
+        <v>44941.72222222222</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2246,7 +2246,7 @@
         <v>91</v>
       </c>
       <c r="C91" s="2">
-        <v>44937.15277777778</v>
+        <v>44941.71875</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2257,7 +2257,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="2">
-        <v>44937.14930555555</v>
+        <v>44941.71527777778</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2268,7 +2268,7 @@
         <v>93</v>
       </c>
       <c r="C93" s="2">
-        <v>44937.14583333334</v>
+        <v>44941.71180555555</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2279,7 +2279,7 @@
         <v>94</v>
       </c>
       <c r="C94" s="2">
-        <v>44937.14236111111</v>
+        <v>44941.70833333334</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2290,7 +2290,7 @@
         <v>95</v>
       </c>
       <c r="C95" s="2">
-        <v>44937.13888888889</v>
+        <v>44941.70486111111</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2301,7 +2301,7 @@
         <v>96</v>
       </c>
       <c r="C96" s="2">
-        <v>44937.13541666666</v>
+        <v>44941.70138888889</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2312,7 +2312,7 @@
         <v>97</v>
       </c>
       <c r="C97" s="2">
-        <v>44937.13194444445</v>
+        <v>44941.69791666666</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2323,7 +2323,7 @@
         <v>98</v>
       </c>
       <c r="C98" s="2">
-        <v>44937.12847222222</v>
+        <v>44941.69444444445</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2334,7 +2334,7 @@
         <v>99</v>
       </c>
       <c r="C99" s="2">
-        <v>44937.125</v>
+        <v>44941.69097222222</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2345,7 +2345,7 @@
         <v>100</v>
       </c>
       <c r="C100" s="2">
-        <v>44937.12152777778</v>
+        <v>44941.6875</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2356,7 +2356,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="2">
-        <v>44937.11805555555</v>
+        <v>44941.68402777778</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2367,7 +2367,7 @@
         <v>102</v>
       </c>
       <c r="C102" s="2">
-        <v>44937.11458333334</v>
+        <v>44941.68055555555</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2378,7 +2378,7 @@
         <v>103</v>
       </c>
       <c r="C103" s="2">
-        <v>44937.11111111111</v>
+        <v>44941.67708333334</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2389,7 +2389,7 @@
         <v>104</v>
       </c>
       <c r="C104" s="2">
-        <v>44937.10763888889</v>
+        <v>44941.67361111111</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2400,7 +2400,7 @@
         <v>105</v>
       </c>
       <c r="C105" s="2">
-        <v>44937.10416666666</v>
+        <v>44941.67013888889</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2411,7 +2411,7 @@
         <v>106</v>
       </c>
       <c r="C106" s="2">
-        <v>44937.10069444445</v>
+        <v>44941.66666666666</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2422,7 +2422,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="2">
-        <v>44937.09722222222</v>
+        <v>44941.66319444445</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2433,7 +2433,7 @@
         <v>108</v>
       </c>
       <c r="C108" s="2">
-        <v>44937.09375</v>
+        <v>44941.65972222222</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2444,7 +2444,7 @@
         <v>109</v>
       </c>
       <c r="C109" s="2">
-        <v>44937.09027777778</v>
+        <v>44941.65625</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2455,7 +2455,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="2">
-        <v>44937.08680555555</v>
+        <v>44941.65277777778</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2466,7 +2466,7 @@
         <v>111</v>
       </c>
       <c r="C111" s="2">
-        <v>44937.08333333334</v>
+        <v>44941.64930555555</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2477,7 +2477,7 @@
         <v>112</v>
       </c>
       <c r="C112" s="2">
-        <v>44937.07986111111</v>
+        <v>44941.64583333334</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2488,7 +2488,7 @@
         <v>113</v>
       </c>
       <c r="C113" s="2">
-        <v>44937.07638888889</v>
+        <v>44941.64236111111</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2499,7 +2499,7 @@
         <v>114</v>
       </c>
       <c r="C114" s="2">
-        <v>44937.07291666666</v>
+        <v>44941.63888888889</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2510,7 +2510,7 @@
         <v>115</v>
       </c>
       <c r="C115" s="2">
-        <v>44937.06944444445</v>
+        <v>44941.63541666666</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2521,7 +2521,7 @@
         <v>116</v>
       </c>
       <c r="C116" s="2">
-        <v>44937.06597222222</v>
+        <v>44941.63194444445</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2532,7 +2532,7 @@
         <v>117</v>
       </c>
       <c r="C117" s="2">
-        <v>44937.0625</v>
+        <v>44941.62847222222</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2543,7 +2543,7 @@
         <v>118</v>
       </c>
       <c r="C118" s="2">
-        <v>44937.05902777778</v>
+        <v>44941.625</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2554,7 +2554,7 @@
         <v>119</v>
       </c>
       <c r="C119" s="2">
-        <v>44937.05555555555</v>
+        <v>44941.62152777778</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2565,7 +2565,7 @@
         <v>120</v>
       </c>
       <c r="C120" s="2">
-        <v>44937.05208333334</v>
+        <v>44941.61805555555</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2576,7 +2576,7 @@
         <v>121</v>
       </c>
       <c r="C121" s="2">
-        <v>44937.04861111111</v>
+        <v>44941.61458333334</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2587,7 +2587,7 @@
         <v>122</v>
       </c>
       <c r="C122" s="2">
-        <v>44937.04513888889</v>
+        <v>44941.61111111111</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2598,7 +2598,7 @@
         <v>123</v>
       </c>
       <c r="C123" s="2">
-        <v>44937.04166666666</v>
+        <v>44941.60763888889</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2609,7 +2609,7 @@
         <v>124</v>
       </c>
       <c r="C124" s="2">
-        <v>44937.03819444445</v>
+        <v>44941.60416666666</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2620,7 +2620,7 @@
         <v>125</v>
       </c>
       <c r="C125" s="2">
-        <v>44937.03472222222</v>
+        <v>44941.60069444445</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2631,7 +2631,7 @@
         <v>126</v>
       </c>
       <c r="C126" s="2">
-        <v>44937.03125</v>
+        <v>44941.59722222222</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2642,7 +2642,7 @@
         <v>127</v>
       </c>
       <c r="C127" s="2">
-        <v>44937.02777777778</v>
+        <v>44941.59375</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2653,7 +2653,7 @@
         <v>128</v>
       </c>
       <c r="C128" s="2">
-        <v>44937.02430555555</v>
+        <v>44941.59027777778</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2664,7 +2664,7 @@
         <v>129</v>
       </c>
       <c r="C129" s="2">
-        <v>44937.02083333334</v>
+        <v>44941.58680555555</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2675,7 +2675,7 @@
         <v>130</v>
       </c>
       <c r="C130" s="2">
-        <v>44937.01736111111</v>
+        <v>44941.58333333334</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2686,7 +2686,7 @@
         <v>131</v>
       </c>
       <c r="C131" s="2">
-        <v>44937.01388888889</v>
+        <v>44941.57986111111</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2697,7 +2697,7 @@
         <v>132</v>
       </c>
       <c r="C132" s="2">
-        <v>44937.01041666666</v>
+        <v>44941.57638888889</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2708,7 +2708,7 @@
         <v>133</v>
       </c>
       <c r="C133" s="2">
-        <v>44937.00694444445</v>
+        <v>44941.57291666666</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2719,7 +2719,7 @@
         <v>134</v>
       </c>
       <c r="C134" s="2">
-        <v>44937.00347222222</v>
+        <v>44941.56944444445</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2730,7 +2730,7 @@
         <v>135</v>
       </c>
       <c r="C135" s="2">
-        <v>44937</v>
+        <v>44941.56597222222</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2741,7 +2741,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="2">
-        <v>44936.99652777778</v>
+        <v>44941.5625</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2752,7 +2752,7 @@
         <v>137</v>
       </c>
       <c r="C137" s="2">
-        <v>44936.99305555555</v>
+        <v>44941.55902777778</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2763,7 +2763,7 @@
         <v>138</v>
       </c>
       <c r="C138" s="2">
-        <v>44936.98958333334</v>
+        <v>44941.55555555555</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2774,7 +2774,7 @@
         <v>139</v>
       </c>
       <c r="C139" s="2">
-        <v>44936.98611111111</v>
+        <v>44941.55208333334</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2785,7 +2785,7 @@
         <v>140</v>
       </c>
       <c r="C140" s="2">
-        <v>44936.98263888889</v>
+        <v>44941.54861111111</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2796,7 +2796,7 @@
         <v>141</v>
       </c>
       <c r="C141" s="2">
-        <v>44936.97916666666</v>
+        <v>44941.54513888889</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2807,7 +2807,7 @@
         <v>142</v>
       </c>
       <c r="C142" s="2">
-        <v>44936.97569444445</v>
+        <v>44941.54166666666</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2818,7 +2818,7 @@
         <v>143</v>
       </c>
       <c r="C143" s="2">
-        <v>44936.97222222222</v>
+        <v>44941.53819444445</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2829,7 +2829,7 @@
         <v>144</v>
       </c>
       <c r="C144" s="2">
-        <v>44936.96875</v>
+        <v>44941.53472222222</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2840,7 +2840,7 @@
         <v>145</v>
       </c>
       <c r="C145" s="2">
-        <v>44936.96527777778</v>
+        <v>44941.53125</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2851,7 +2851,7 @@
         <v>146</v>
       </c>
       <c r="C146" s="2">
-        <v>44936.96180555555</v>
+        <v>44941.52777777778</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2862,7 +2862,7 @@
         <v>147</v>
       </c>
       <c r="C147" s="2">
-        <v>44936.95833333334</v>
+        <v>44941.52430555555</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2873,7 +2873,7 @@
         <v>148</v>
       </c>
       <c r="C148" s="2">
-        <v>44936.95486111111</v>
+        <v>44941.52083333334</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2884,7 +2884,7 @@
         <v>149</v>
       </c>
       <c r="C149" s="2">
-        <v>44936.95138888889</v>
+        <v>44941.51736111111</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2895,7 +2895,7 @@
         <v>150</v>
       </c>
       <c r="C150" s="2">
-        <v>44936.94791666666</v>
+        <v>44941.51388888889</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2906,7 +2906,7 @@
         <v>151</v>
       </c>
       <c r="C151" s="2">
-        <v>44936.94444444445</v>
+        <v>44941.51041666666</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2917,7 +2917,7 @@
         <v>152</v>
       </c>
       <c r="C152" s="2">
-        <v>44936.94097222222</v>
+        <v>44941.50694444445</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2928,7 +2928,7 @@
         <v>153</v>
       </c>
       <c r="C153" s="2">
-        <v>44936.9375</v>
+        <v>44941.50347222222</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2939,7 +2939,7 @@
         <v>154</v>
       </c>
       <c r="C154" s="2">
-        <v>44936.93402777778</v>
+        <v>44941.5</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2950,7 +2950,7 @@
         <v>155</v>
       </c>
       <c r="C155" s="2">
-        <v>44936.93055555555</v>
+        <v>44941.49652777778</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2961,7 +2961,7 @@
         <v>156</v>
       </c>
       <c r="C156" s="2">
-        <v>44936.92708333334</v>
+        <v>44941.49305555555</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2972,7 +2972,7 @@
         <v>157</v>
       </c>
       <c r="C157" s="2">
-        <v>44936.92361111111</v>
+        <v>44941.48958333334</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2983,7 +2983,7 @@
         <v>158</v>
       </c>
       <c r="C158" s="2">
-        <v>44936.92013888889</v>
+        <v>44941.48611111111</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2994,7 +2994,7 @@
         <v>159</v>
       </c>
       <c r="C159" s="2">
-        <v>44936.91666666666</v>
+        <v>44941.48263888889</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -3005,7 +3005,7 @@
         <v>160</v>
       </c>
       <c r="C160" s="2">
-        <v>44936.91319444445</v>
+        <v>44941.47916666666</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -3016,7 +3016,7 @@
         <v>161</v>
       </c>
       <c r="C161" s="2">
-        <v>44936.90972222222</v>
+        <v>44941.47569444445</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -3027,7 +3027,7 @@
         <v>162</v>
       </c>
       <c r="C162" s="2">
-        <v>44936.90625</v>
+        <v>44941.47222222222</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3038,7 +3038,7 @@
         <v>163</v>
       </c>
       <c r="C163" s="2">
-        <v>44936.90277777778</v>
+        <v>44941.46875</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3049,7 +3049,7 @@
         <v>164</v>
       </c>
       <c r="C164" s="2">
-        <v>44936.89930555555</v>
+        <v>44941.46527777778</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3060,7 +3060,7 @@
         <v>165</v>
       </c>
       <c r="C165" s="2">
-        <v>44936.89583333334</v>
+        <v>44941.46180555555</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3071,7 +3071,7 @@
         <v>166</v>
       </c>
       <c r="C166" s="2">
-        <v>44936.89236111111</v>
+        <v>44941.45833333334</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3082,7 +3082,7 @@
         <v>167</v>
       </c>
       <c r="C167" s="2">
-        <v>44936.88888888889</v>
+        <v>44941.45486111111</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3093,7 +3093,7 @@
         <v>168</v>
       </c>
       <c r="C168" s="2">
-        <v>44936.88541666666</v>
+        <v>44941.45138888889</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3104,7 +3104,7 @@
         <v>169</v>
       </c>
       <c r="C169" s="2">
-        <v>44936.88194444445</v>
+        <v>44941.44791666666</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3115,7 +3115,7 @@
         <v>170</v>
       </c>
       <c r="C170" s="2">
-        <v>44936.87847222222</v>
+        <v>44941.44444444445</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3126,7 +3126,7 @@
         <v>171</v>
       </c>
       <c r="C171" s="2">
-        <v>44936.875</v>
+        <v>44941.44097222222</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3137,7 +3137,7 @@
         <v>172</v>
       </c>
       <c r="C172" s="2">
-        <v>44936.87152777778</v>
+        <v>44941.4375</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3148,7 +3148,7 @@
         <v>173</v>
       </c>
       <c r="C173" s="2">
-        <v>44936.86805555555</v>
+        <v>44941.43402777778</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3159,7 +3159,7 @@
         <v>174</v>
       </c>
       <c r="C174" s="2">
-        <v>44936.86458333334</v>
+        <v>44941.43055555555</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3170,7 +3170,7 @@
         <v>175</v>
       </c>
       <c r="C175" s="2">
-        <v>44936.86111111111</v>
+        <v>44941.42708333334</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3181,7 +3181,7 @@
         <v>176</v>
       </c>
       <c r="C176" s="2">
-        <v>44936.85763888889</v>
+        <v>44941.42361111111</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3192,7 +3192,7 @@
         <v>177</v>
       </c>
       <c r="C177" s="2">
-        <v>44936.85416666666</v>
+        <v>44941.42013888889</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3203,7 +3203,7 @@
         <v>178</v>
       </c>
       <c r="C178" s="2">
-        <v>44936.85069444445</v>
+        <v>44941.41666666666</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3214,7 +3214,7 @@
         <v>179</v>
       </c>
       <c r="C179" s="2">
-        <v>44936.84722222222</v>
+        <v>44941.41319444445</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3225,7 +3225,7 @@
         <v>180</v>
       </c>
       <c r="C180" s="2">
-        <v>44936.84375</v>
+        <v>44941.40972222222</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3236,7 +3236,7 @@
         <v>181</v>
       </c>
       <c r="C181" s="2">
-        <v>44936.84027777778</v>
+        <v>44941.40625</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3247,7 +3247,7 @@
         <v>182</v>
       </c>
       <c r="C182" s="2">
-        <v>44936.83680555555</v>
+        <v>44941.40277777778</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3258,7 +3258,7 @@
         <v>183</v>
       </c>
       <c r="C183" s="2">
-        <v>44936.83333333334</v>
+        <v>44941.39930555555</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3269,7 +3269,7 @@
         <v>184</v>
       </c>
       <c r="C184" s="2">
-        <v>44936.82986111111</v>
+        <v>44941.39583333334</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3280,7 +3280,7 @@
         <v>185</v>
       </c>
       <c r="C185" s="2">
-        <v>44936.82638888889</v>
+        <v>44941.39236111111</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3291,7 +3291,7 @@
         <v>186</v>
       </c>
       <c r="C186" s="2">
-        <v>44936.82291666666</v>
+        <v>44941.38888888889</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3302,7 +3302,7 @@
         <v>187</v>
       </c>
       <c r="C187" s="2">
-        <v>44936.81944444445</v>
+        <v>44941.38541666666</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3313,7 +3313,7 @@
         <v>188</v>
       </c>
       <c r="C188" s="2">
-        <v>44936.81597222222</v>
+        <v>44941.38194444445</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3324,7 +3324,7 @@
         <v>189</v>
       </c>
       <c r="C189" s="2">
-        <v>44936.8125</v>
+        <v>44941.37847222222</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3335,7 +3335,7 @@
         <v>190</v>
       </c>
       <c r="C190" s="2">
-        <v>44936.80902777778</v>
+        <v>44941.375</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3346,7 +3346,7 @@
         <v>191</v>
       </c>
       <c r="C191" s="2">
-        <v>44936.80555555555</v>
+        <v>44941.37152777778</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3357,7 +3357,7 @@
         <v>192</v>
       </c>
       <c r="C192" s="2">
-        <v>44936.80208333334</v>
+        <v>44941.36805555555</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3368,7 +3368,7 @@
         <v>193</v>
       </c>
       <c r="C193" s="2">
-        <v>44936.79861111111</v>
+        <v>44941.36458333334</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3379,7 +3379,7 @@
         <v>194</v>
       </c>
       <c r="C194" s="2">
-        <v>44936.79513888889</v>
+        <v>44941.36111111111</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3390,7 +3390,7 @@
         <v>195</v>
       </c>
       <c r="C195" s="2">
-        <v>44936.79166666666</v>
+        <v>44941.35763888889</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3401,7 +3401,7 @@
         <v>196</v>
       </c>
       <c r="C196" s="2">
-        <v>44936.78819444445</v>
+        <v>44941.35416666666</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3412,7 +3412,7 @@
         <v>197</v>
       </c>
       <c r="C197" s="2">
-        <v>44936.78472222222</v>
+        <v>44941.35069444445</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3423,7 +3423,7 @@
         <v>198</v>
       </c>
       <c r="C198" s="2">
-        <v>44936.78125</v>
+        <v>44941.34722222222</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3434,7 +3434,7 @@
         <v>199</v>
       </c>
       <c r="C199" s="2">
-        <v>44936.77777777778</v>
+        <v>44941.34375</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3445,7 +3445,7 @@
         <v>200</v>
       </c>
       <c r="C200" s="2">
-        <v>44936.77430555555</v>
+        <v>44941.34027777778</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3456,7 +3456,7 @@
         <v>201</v>
       </c>
       <c r="C201" s="2">
-        <v>44936.77083333334</v>
+        <v>44941.33680555555</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3467,7 +3467,7 @@
         <v>202</v>
       </c>
       <c r="C202" s="2">
-        <v>44936.76736111111</v>
+        <v>44941.33333333334</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3478,7 +3478,7 @@
         <v>203</v>
       </c>
       <c r="C203" s="2">
-        <v>44936.76388888889</v>
+        <v>44941.32986111111</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3489,7 +3489,7 @@
         <v>204</v>
       </c>
       <c r="C204" s="2">
-        <v>44936.76041666666</v>
+        <v>44941.32638888889</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3500,7 +3500,7 @@
         <v>205</v>
       </c>
       <c r="C205" s="2">
-        <v>44936.75694444445</v>
+        <v>44941.32291666666</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3511,7 +3511,7 @@
         <v>206</v>
       </c>
       <c r="C206" s="2">
-        <v>44936.75347222222</v>
+        <v>44941.31944444445</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3522,7 +3522,7 @@
         <v>207</v>
       </c>
       <c r="C207" s="2">
-        <v>44936.75</v>
+        <v>44941.31597222222</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3533,7 +3533,7 @@
         <v>208</v>
       </c>
       <c r="C208" s="2">
-        <v>44936.74652777778</v>
+        <v>44941.3125</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3544,7 +3544,7 @@
         <v>209</v>
       </c>
       <c r="C209" s="2">
-        <v>44936.74305555555</v>
+        <v>44941.30902777778</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3555,7 +3555,7 @@
         <v>210</v>
       </c>
       <c r="C210" s="2">
-        <v>44936.73958333334</v>
+        <v>44941.30555555555</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3566,7 +3566,7 @@
         <v>211</v>
       </c>
       <c r="C211" s="2">
-        <v>44936.73611111111</v>
+        <v>44941.30208333334</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3577,7 +3577,7 @@
         <v>212</v>
       </c>
       <c r="C212" s="2">
-        <v>44936.73263888889</v>
+        <v>44941.29861111111</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3588,7 +3588,7 @@
         <v>213</v>
       </c>
       <c r="C213" s="2">
-        <v>44936.72916666666</v>
+        <v>44941.29513888889</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3599,7 +3599,7 @@
         <v>214</v>
       </c>
       <c r="C214" s="2">
-        <v>44936.72569444445</v>
+        <v>44941.29166666666</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3610,7 +3610,7 @@
         <v>215</v>
       </c>
       <c r="C215" s="2">
-        <v>44936.72222222222</v>
+        <v>44941.28819444445</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3621,7 +3621,7 @@
         <v>216</v>
       </c>
       <c r="C216" s="2">
-        <v>44936.71875</v>
+        <v>44941.28472222222</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3632,7 +3632,7 @@
         <v>217</v>
       </c>
       <c r="C217" s="2">
-        <v>44936.71527777778</v>
+        <v>44941.28125</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3643,7 +3643,7 @@
         <v>218</v>
       </c>
       <c r="C218" s="2">
-        <v>44936.71180555555</v>
+        <v>44941.27777777778</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3654,7 +3654,7 @@
         <v>219</v>
       </c>
       <c r="C219" s="2">
-        <v>44936.70833333334</v>
+        <v>44941.27430555555</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3665,7 +3665,7 @@
         <v>220</v>
       </c>
       <c r="C220" s="2">
-        <v>44936.70486111111</v>
+        <v>44941.27083333334</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3676,7 +3676,7 @@
         <v>221</v>
       </c>
       <c r="C221" s="2">
-        <v>44936.70138888889</v>
+        <v>44941.26736111111</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3687,7 +3687,7 @@
         <v>222</v>
       </c>
       <c r="C222" s="2">
-        <v>44936.69791666666</v>
+        <v>44941.26388888889</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3698,7 +3698,7 @@
         <v>223</v>
       </c>
       <c r="C223" s="2">
-        <v>44936.69444444445</v>
+        <v>44941.26041666666</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3709,7 +3709,7 @@
         <v>224</v>
       </c>
       <c r="C224" s="2">
-        <v>44936.69097222222</v>
+        <v>44941.25694444445</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3720,7 +3720,7 @@
         <v>225</v>
       </c>
       <c r="C225" s="2">
-        <v>44936.6875</v>
+        <v>44941.25347222222</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3731,7 +3731,7 @@
         <v>226</v>
       </c>
       <c r="C226" s="2">
-        <v>44936.68402777778</v>
+        <v>44941.25</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3742,7 +3742,7 @@
         <v>227</v>
       </c>
       <c r="C227" s="2">
-        <v>44936.68055555555</v>
+        <v>44941.24652777778</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3753,7 +3753,7 @@
         <v>228</v>
       </c>
       <c r="C228" s="2">
-        <v>44936.67708333334</v>
+        <v>44941.24305555555</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3764,7 +3764,7 @@
         <v>229</v>
       </c>
       <c r="C229" s="2">
-        <v>44936.67361111111</v>
+        <v>44941.23958333334</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3775,7 +3775,7 @@
         <v>230</v>
       </c>
       <c r="C230" s="2">
-        <v>44936.67013888889</v>
+        <v>44941.23611111111</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3786,7 +3786,7 @@
         <v>231</v>
       </c>
       <c r="C231" s="2">
-        <v>44936.66666666666</v>
+        <v>44941.23263888889</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3797,7 +3797,7 @@
         <v>232</v>
       </c>
       <c r="C232" s="2">
-        <v>44936.66319444445</v>
+        <v>44941.22916666666</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3808,7 +3808,7 @@
         <v>233</v>
       </c>
       <c r="C233" s="2">
-        <v>44936.65972222222</v>
+        <v>44941.22569444445</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3819,7 +3819,7 @@
         <v>234</v>
       </c>
       <c r="C234" s="2">
-        <v>44936.65625</v>
+        <v>44941.22222222222</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3830,7 +3830,7 @@
         <v>235</v>
       </c>
       <c r="C235" s="2">
-        <v>44936.65277777778</v>
+        <v>44941.21875</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3841,7 +3841,7 @@
         <v>236</v>
       </c>
       <c r="C236" s="2">
-        <v>44936.64930555555</v>
+        <v>44941.21527777778</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3852,7 +3852,7 @@
         <v>237</v>
       </c>
       <c r="C237" s="2">
-        <v>44936.64583333334</v>
+        <v>44941.21180555555</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3863,7 +3863,7 @@
         <v>238</v>
       </c>
       <c r="C238" s="2">
-        <v>44936.64236111111</v>
+        <v>44941.20833333334</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3874,7 +3874,7 @@
         <v>239</v>
       </c>
       <c r="C239" s="2">
-        <v>44936.63888888889</v>
+        <v>44941.20486111111</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3885,7 +3885,7 @@
         <v>240</v>
       </c>
       <c r="C240" s="2">
-        <v>44936.63541666666</v>
+        <v>44941.20138888889</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3896,7 +3896,7 @@
         <v>241</v>
       </c>
       <c r="C241" s="2">
-        <v>44936.63194444445</v>
+        <v>44941.19791666666</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3907,7 +3907,7 @@
         <v>242</v>
       </c>
       <c r="C242" s="2">
-        <v>44936.62847222222</v>
+        <v>44941.19444444445</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3918,7 +3918,7 @@
         <v>243</v>
       </c>
       <c r="C243" s="2">
-        <v>44936.625</v>
+        <v>44941.19097222222</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3929,7 +3929,7 @@
         <v>244</v>
       </c>
       <c r="C244" s="2">
-        <v>44936.62152777778</v>
+        <v>44941.1875</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3940,7 +3940,7 @@
         <v>245</v>
       </c>
       <c r="C245" s="2">
-        <v>44936.61805555555</v>
+        <v>44941.18402777778</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3951,7 +3951,7 @@
         <v>246</v>
       </c>
       <c r="C246" s="2">
-        <v>44936.61458333334</v>
+        <v>44941.18055555555</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3962,7 +3962,7 @@
         <v>247</v>
       </c>
       <c r="C247" s="2">
-        <v>44936.61111111111</v>
+        <v>44941.17708333334</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3973,7 +3973,7 @@
         <v>248</v>
       </c>
       <c r="C248" s="2">
-        <v>44936.60763888889</v>
+        <v>44941.17361111111</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3984,7 +3984,7 @@
         <v>249</v>
       </c>
       <c r="C249" s="2">
-        <v>44936.60416666666</v>
+        <v>44941.17013888889</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3995,7 +3995,7 @@
         <v>250</v>
       </c>
       <c r="C250" s="2">
-        <v>44936.60069444445</v>
+        <v>44941.16666666666</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -4006,7 +4006,7 @@
         <v>251</v>
       </c>
       <c r="C251" s="2">
-        <v>44936.59722222222</v>
+        <v>44941.16319444445</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -4017,7 +4017,7 @@
         <v>252</v>
       </c>
       <c r="C252" s="2">
-        <v>44936.59375</v>
+        <v>44941.15972222222</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -4028,7 +4028,7 @@
         <v>253</v>
       </c>
       <c r="C253" s="2">
-        <v>44936.59027777778</v>
+        <v>44941.15625</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -4039,7 +4039,7 @@
         <v>254</v>
       </c>
       <c r="C254" s="2">
-        <v>44936.58680555555</v>
+        <v>44941.15277777778</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -4050,7 +4050,7 @@
         <v>255</v>
       </c>
       <c r="C255" s="2">
-        <v>44936.58333333334</v>
+        <v>44941.14930555555</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -4061,7 +4061,7 @@
         <v>256</v>
       </c>
       <c r="C256" s="2">
-        <v>44936.57986111111</v>
+        <v>44941.14583333334</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -4072,7 +4072,7 @@
         <v>257</v>
       </c>
       <c r="C257" s="2">
-        <v>44936.57638888889</v>
+        <v>44941.14236111111</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -4083,7 +4083,7 @@
         <v>258</v>
       </c>
       <c r="C258" s="2">
-        <v>44936.57291666666</v>
+        <v>44941.13888888889</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -4094,7 +4094,7 @@
         <v>259</v>
       </c>
       <c r="C259" s="2">
-        <v>44936.56944444445</v>
+        <v>44941.13541666666</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -4105,7 +4105,7 @@
         <v>260</v>
       </c>
       <c r="C260" s="2">
-        <v>44936.56597222222</v>
+        <v>44941.13194444445</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -4116,7 +4116,7 @@
         <v>261</v>
       </c>
       <c r="C261" s="2">
-        <v>44936.5625</v>
+        <v>44941.12847222222</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -4127,7 +4127,7 @@
         <v>262</v>
       </c>
       <c r="C262" s="2">
-        <v>44936.55902777778</v>
+        <v>44941.125</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -4138,7 +4138,7 @@
         <v>263</v>
       </c>
       <c r="C263" s="2">
-        <v>44936.55555555555</v>
+        <v>44941.12152777778</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -4149,7 +4149,7 @@
         <v>264</v>
       </c>
       <c r="C264" s="2">
-        <v>44936.55208333334</v>
+        <v>44941.11805555555</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -4160,7 +4160,7 @@
         <v>265</v>
       </c>
       <c r="C265" s="2">
-        <v>44936.54861111111</v>
+        <v>44941.11458333334</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -4171,7 +4171,7 @@
         <v>266</v>
       </c>
       <c r="C266" s="2">
-        <v>44936.54513888889</v>
+        <v>44941.11111111111</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -4182,7 +4182,7 @@
         <v>267</v>
       </c>
       <c r="C267" s="2">
-        <v>44936.54166666666</v>
+        <v>44941.10763888889</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -4193,7 +4193,7 @@
         <v>268</v>
       </c>
       <c r="C268" s="2">
-        <v>44936.53819444445</v>
+        <v>44941.10416666666</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -4204,7 +4204,7 @@
         <v>269</v>
       </c>
       <c r="C269" s="2">
-        <v>44936.53472222222</v>
+        <v>44941.10069444445</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -4215,7 +4215,7 @@
         <v>270</v>
       </c>
       <c r="C270" s="2">
-        <v>44936.53125</v>
+        <v>44941.09722222222</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -4226,7 +4226,7 @@
         <v>271</v>
       </c>
       <c r="C271" s="2">
-        <v>44936.52777777778</v>
+        <v>44941.09375</v>
       </c>
     </row>
     <row r="272" spans="1:3">
@@ -4237,7 +4237,7 @@
         <v>272</v>
       </c>
       <c r="C272" s="2">
-        <v>44936.52430555555</v>
+        <v>44941.09027777778</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -4248,7 +4248,7 @@
         <v>273</v>
       </c>
       <c r="C273" s="2">
-        <v>44936.52083333334</v>
+        <v>44941.08680555555</v>
       </c>
     </row>
     <row r="274" spans="1:3">
@@ -4259,7 +4259,7 @@
         <v>274</v>
       </c>
       <c r="C274" s="2">
-        <v>44936.51736111111</v>
+        <v>44941.08333333334</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -4270,7 +4270,7 @@
         <v>275</v>
       </c>
       <c r="C275" s="2">
-        <v>44936.51388888889</v>
+        <v>44941.07986111111</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -4281,7 +4281,7 @@
         <v>276</v>
       </c>
       <c r="C276" s="2">
-        <v>44936.51041666666</v>
+        <v>44941.07638888889</v>
       </c>
     </row>
     <row r="277" spans="1:3">
@@ -4292,7 +4292,7 @@
         <v>277</v>
       </c>
       <c r="C277" s="2">
-        <v>44936.50694444445</v>
+        <v>44941.07291666666</v>
       </c>
     </row>
     <row r="278" spans="1:3">
@@ -4303,7 +4303,7 @@
         <v>278</v>
       </c>
       <c r="C278" s="2">
-        <v>44936.50347222222</v>
+        <v>44941.06944444445</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -4314,7 +4314,7 @@
         <v>279</v>
       </c>
       <c r="C279" s="2">
-        <v>44936.5</v>
+        <v>44941.06597222222</v>
       </c>
     </row>
     <row r="280" spans="1:3">
@@ -4325,7 +4325,7 @@
         <v>280</v>
       </c>
       <c r="C280" s="2">
-        <v>44936.49652777778</v>
+        <v>44941.0625</v>
       </c>
     </row>
     <row r="281" spans="1:3">
@@ -4336,7 +4336,7 @@
         <v>281</v>
       </c>
       <c r="C281" s="2">
-        <v>44936.49305555555</v>
+        <v>44941.05902777778</v>
       </c>
     </row>
     <row r="282" spans="1:3">
@@ -4347,7 +4347,7 @@
         <v>282</v>
       </c>
       <c r="C282" s="2">
-        <v>44936.48958333334</v>
+        <v>44941.05555555555</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -4358,7 +4358,7 @@
         <v>283</v>
       </c>
       <c r="C283" s="2">
-        <v>44936.48611111111</v>
+        <v>44941.05208333334</v>
       </c>
     </row>
     <row r="284" spans="1:3">
@@ -4369,7 +4369,7 @@
         <v>284</v>
       </c>
       <c r="C284" s="2">
-        <v>44936.48263888889</v>
+        <v>44941.04861111111</v>
       </c>
     </row>
     <row r="285" spans="1:3">
@@ -4380,7 +4380,7 @@
         <v>285</v>
       </c>
       <c r="C285" s="2">
-        <v>44936.47916666666</v>
+        <v>44941.04513888889</v>
       </c>
     </row>
     <row r="286" spans="1:3">
@@ -4391,7 +4391,7 @@
         <v>286</v>
       </c>
       <c r="C286" s="2">
-        <v>44936.47569444445</v>
+        <v>44941.04166666666</v>
       </c>
     </row>
     <row r="287" spans="1:3">
@@ -4402,7 +4402,7 @@
         <v>287</v>
       </c>
       <c r="C287" s="2">
-        <v>44936.47222222222</v>
+        <v>44941.03819444445</v>
       </c>
     </row>
     <row r="288" spans="1:3">
@@ -4413,7 +4413,7 @@
         <v>288</v>
       </c>
       <c r="C288" s="2">
-        <v>44936.46875</v>
+        <v>44941.03472222222</v>
       </c>
     </row>
     <row r="289" spans="1:3">
@@ -4424,7 +4424,7 @@
         <v>289</v>
       </c>
       <c r="C289" s="2">
-        <v>44936.46527777778</v>
+        <v>44941.03125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>